<commit_message>
Description to post alarms 20240424_1
</commit_message>
<xml_diff>
--- a/CMS/excel_exports/post/post_alarms_20240424.xlsx
+++ b/CMS/excel_exports/post/post_alarms_20240424.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SergioPaniagua\Documents\CMS_Testing\CMS\excel_exports\post\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816EC7A6-5CEB-4028-B905-3F617B97DD2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5936E8C-8870-43C9-B166-375C9B608359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24960" yWindow="-18120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$280</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$280</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1774" uniqueCount="801">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="810">
   <si>
     <t>Severity</t>
   </si>
@@ -2426,6 +2426,33 @@
   </si>
   <si>
     <t>CYP holding doors open on site</t>
+  </si>
+  <si>
+    <t>PED being used for access</t>
+  </si>
+  <si>
+    <t>PSD opening</t>
+  </si>
+  <si>
+    <t>General fault alarm as a result of loss of power</t>
+  </si>
+  <si>
+    <t>Door forced open</t>
+  </si>
+  <si>
+    <t>Isolation of lift causes this alarm</t>
+  </si>
+  <si>
+    <t>PSD isolated during a blockade</t>
+  </si>
+  <si>
+    <t>Isolation of panel</t>
+  </si>
+  <si>
+    <t>Not currently connected to Sunshine</t>
+  </si>
+  <si>
+    <t>Real alarm to be looked at</t>
   </si>
 </sst>
 </file>
@@ -2497,7 +2524,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2805,8 +2832,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2821,6 +2848,7 @@
     <col min="8" max="8" width="21.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -3021,6 +3049,9 @@
       <c r="J8" t="s">
         <v>36</v>
       </c>
+      <c r="K8" t="s">
+        <v>803</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -3044,6 +3075,9 @@
       <c r="J9" t="s">
         <v>36</v>
       </c>
+      <c r="K9" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -3066,6 +3100,9 @@
       </c>
       <c r="J10" t="s">
         <v>36</v>
+      </c>
+      <c r="K10" t="s">
+        <v>804</v>
       </c>
     </row>
     <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -3206,7 +3243,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>231</v>
       </c>
@@ -3228,8 +3265,11 @@
       <c r="J17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K17" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>231</v>
       </c>
@@ -3251,8 +3291,11 @@
       <c r="J18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K18" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -3275,7 +3318,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -3298,7 +3341,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -3321,7 +3364,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -3344,7 +3387,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -3367,7 +3410,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -3390,7 +3433,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -3413,7 +3456,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -3436,7 +3479,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -3459,7 +3502,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -3482,7 +3525,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -3505,7 +3548,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -3528,7 +3571,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -3551,7 +3594,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -3574,7 +3617,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -3597,7 +3640,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -3620,7 +3663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -3643,7 +3686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -3666,7 +3709,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -3689,7 +3732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>231</v>
       </c>
@@ -3711,8 +3754,11 @@
       <c r="J38" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K38" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -3734,8 +3780,11 @@
       <c r="J39" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K39" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>133</v>
       </c>
@@ -3758,7 +3807,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>133</v>
       </c>
@@ -3781,7 +3830,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>133</v>
       </c>
@@ -3804,7 +3853,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>133</v>
       </c>
@@ -3827,7 +3876,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>133</v>
       </c>
@@ -3850,7 +3899,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>133</v>
       </c>
@@ -3873,7 +3922,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>133</v>
       </c>
@@ -3896,7 +3945,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -3918,8 +3967,11 @@
       <c r="J47" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K47" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>231</v>
       </c>
@@ -3941,8 +3993,11 @@
       <c r="J48" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K48" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>231</v>
       </c>
@@ -3964,8 +4019,11 @@
       <c r="J49" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K49" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>133</v>
       </c>
@@ -3988,7 +4046,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>133</v>
       </c>
@@ -4011,7 +4069,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>133</v>
       </c>
@@ -4034,7 +4092,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>133</v>
       </c>
@@ -4057,7 +4115,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>231</v>
       </c>
@@ -4079,8 +4137,11 @@
       <c r="J54" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K54" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>133</v>
       </c>
@@ -4103,7 +4164,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>133</v>
       </c>
@@ -4126,7 +4187,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>133</v>
       </c>
@@ -4149,7 +4210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>133</v>
       </c>
@@ -4172,7 +4233,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>133</v>
       </c>
@@ -4195,7 +4256,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>231</v>
       </c>
@@ -4217,8 +4278,11 @@
       <c r="J60" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K60" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>771</v>
       </c>
@@ -4246,8 +4310,11 @@
       <c r="J61" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K61" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>133</v>
       </c>
@@ -4270,7 +4337,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>133</v>
       </c>
@@ -4293,7 +4360,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>133</v>
       </c>
@@ -5052,7 +5119,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>231</v>
       </c>
@@ -5075,7 +5142,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>231</v>
       </c>
@@ -5098,7 +5165,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>231</v>
       </c>
@@ -5121,7 +5188,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>231</v>
       </c>
@@ -5144,7 +5211,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>231</v>
       </c>
@@ -5167,7 +5234,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>231</v>
       </c>
@@ -5190,7 +5257,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>231</v>
       </c>
@@ -5213,7 +5280,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>231</v>
       </c>
@@ -5236,7 +5303,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>231</v>
       </c>
@@ -5259,7 +5326,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>231</v>
       </c>
@@ -5282,7 +5349,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>231</v>
       </c>
@@ -5305,7 +5372,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>231</v>
       </c>
@@ -5328,7 +5395,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>231</v>
       </c>
@@ -5351,7 +5418,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>133</v>
       </c>
@@ -5374,7 +5441,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>10</v>
       </c>
@@ -5396,8 +5463,11 @@
       <c r="J111" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K111" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>231</v>
       </c>
@@ -5420,7 +5490,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>10</v>
       </c>
@@ -5442,8 +5512,11 @@
       <c r="J113" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K113" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>231</v>
       </c>
@@ -5465,8 +5538,11 @@
       <c r="J114" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K114" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>231</v>
       </c>
@@ -5488,8 +5564,11 @@
       <c r="J115" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K115" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>231</v>
       </c>
@@ -5512,7 +5591,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>231</v>
       </c>
@@ -5535,7 +5614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>231</v>
       </c>
@@ -5557,8 +5636,11 @@
       <c r="J118" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K118" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>231</v>
       </c>
@@ -5581,7 +5663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>231</v>
       </c>
@@ -5604,7 +5686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>231</v>
       </c>
@@ -5627,7 +5709,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>231</v>
       </c>
@@ -5650,7 +5732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>231</v>
       </c>
@@ -5673,7 +5755,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>231</v>
       </c>
@@ -5696,7 +5778,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>231</v>
       </c>
@@ -5719,7 +5801,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>231</v>
       </c>
@@ -5742,7 +5824,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>231</v>
       </c>
@@ -5765,7 +5847,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>231</v>
       </c>
@@ -6156,7 +6238,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="145" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>231</v>
       </c>
@@ -6179,7 +6261,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>231</v>
       </c>
@@ -6201,8 +6283,11 @@
       <c r="J146" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K146" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>231</v>
       </c>
@@ -6224,8 +6309,11 @@
       <c r="J147" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K147" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>231</v>
       </c>
@@ -6247,8 +6335,11 @@
       <c r="J148" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K148" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>231</v>
       </c>
@@ -6270,8 +6361,11 @@
       <c r="J149" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="150" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K149" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>231</v>
       </c>
@@ -6294,7 +6388,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>231</v>
       </c>
@@ -6317,7 +6411,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="152" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>231</v>
       </c>
@@ -6340,7 +6434,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="153" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>231</v>
       </c>
@@ -6363,7 +6457,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="154" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>231</v>
       </c>
@@ -6386,7 +6480,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="155" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>231</v>
       </c>
@@ -6409,7 +6503,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="156" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>231</v>
       </c>
@@ -6432,7 +6526,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="157" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>231</v>
       </c>
@@ -6455,7 +6549,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="158" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>231</v>
       </c>
@@ -6478,7 +6572,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="159" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>231</v>
       </c>
@@ -6501,7 +6595,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="160" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>231</v>
       </c>
@@ -6524,7 +6618,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>231</v>
       </c>
@@ -6547,7 +6641,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>231</v>
       </c>
@@ -6570,7 +6664,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>231</v>
       </c>
@@ -6593,7 +6687,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>231</v>
       </c>
@@ -6616,7 +6710,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>231</v>
       </c>
@@ -6639,7 +6733,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>231</v>
       </c>
@@ -6662,7 +6756,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>231</v>
       </c>
@@ -6685,7 +6779,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>10</v>
       </c>
@@ -6707,8 +6801,11 @@
       <c r="J168" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K168" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>231</v>
       </c>
@@ -6730,8 +6827,11 @@
       <c r="J169" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K169" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>231</v>
       </c>
@@ -6753,8 +6853,11 @@
       <c r="J170" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K170" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>231</v>
       </c>
@@ -6776,8 +6879,11 @@
       <c r="J171" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K171" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>231</v>
       </c>
@@ -6799,8 +6905,11 @@
       <c r="J172" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K172" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>10</v>
       </c>
@@ -6822,8 +6931,11 @@
       <c r="J173" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K173" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>231</v>
       </c>
@@ -6846,7 +6958,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>231</v>
       </c>
@@ -6869,7 +6981,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>231</v>
       </c>
@@ -6892,7 +7004,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="177" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>231</v>
       </c>
@@ -6915,7 +7027,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="178" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>231</v>
       </c>
@@ -6938,7 +7050,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>231</v>
       </c>
@@ -6961,7 +7073,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="180" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>231</v>
       </c>
@@ -6984,7 +7096,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="181" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>231</v>
       </c>
@@ -7007,7 +7119,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="182" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>231</v>
       </c>
@@ -7030,7 +7142,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="183" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>231</v>
       </c>
@@ -7053,7 +7165,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="184" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>231</v>
       </c>
@@ -7076,7 +7188,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>231</v>
       </c>
@@ -7098,8 +7210,11 @@
       <c r="J185" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K185" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>231</v>
       </c>
@@ -7121,8 +7236,11 @@
       <c r="J186" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K186" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>231</v>
       </c>
@@ -7144,8 +7262,11 @@
       <c r="J187" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K187" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>133</v>
       </c>
@@ -7167,8 +7288,11 @@
       <c r="J188" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K188" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>10</v>
       </c>
@@ -7190,8 +7314,11 @@
       <c r="J189" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K189" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>10</v>
       </c>
@@ -7213,8 +7340,11 @@
       <c r="J190" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K190" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>133</v>
       </c>
@@ -7237,7 +7367,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="192" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>231</v>
       </c>
@@ -8852,7 +8982,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>133</v>
       </c>
@@ -8875,7 +9005,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>713</v>
       </c>
@@ -8903,8 +9033,11 @@
       <c r="J258" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K258" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="259" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>713</v>
       </c>
@@ -8932,8 +9065,11 @@
       <c r="J259" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K259" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="260" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>713</v>
       </c>
@@ -8961,8 +9097,11 @@
       <c r="J260" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K260" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="261" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>713</v>
       </c>
@@ -8990,8 +9129,11 @@
       <c r="J261" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K261" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="262" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>771</v>
       </c>
@@ -9019,8 +9161,11 @@
       <c r="J262" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="263" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K262" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="263" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>713</v>
       </c>
@@ -9049,7 +9194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="264" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>713</v>
       </c>
@@ -9078,7 +9223,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="265" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>713</v>
       </c>
@@ -9107,7 +9252,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="266" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>713</v>
       </c>
@@ -9136,7 +9281,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="267" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>713</v>
       </c>
@@ -9165,7 +9310,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="268" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>713</v>
       </c>
@@ -9194,7 +9339,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="269" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>713</v>
       </c>
@@ -9223,7 +9368,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="270" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>713</v>
       </c>
@@ -9252,7 +9397,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="271" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>713</v>
       </c>
@@ -9281,7 +9426,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="272" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>713</v>
       </c>
@@ -9310,7 +9455,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="273" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>771</v>
       </c>
@@ -9339,7 +9484,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="274" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>771</v>
       </c>
@@ -9368,7 +9513,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="275" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>771</v>
       </c>
@@ -9397,7 +9542,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="276" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>771</v>
       </c>
@@ -9426,7 +9571,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>771</v>
       </c>
@@ -9454,8 +9599,11 @@
       <c r="J277" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="278" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K277" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="278" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>771</v>
       </c>
@@ -9484,7 +9632,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>713</v>
       </c>
@@ -9512,8 +9660,11 @@
       <c r="J279" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K279" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="280" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>713</v>
       </c>
@@ -9543,15 +9694,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J280" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:K280" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="9">
       <filters>
         <filter val="ARN"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:J280">
-      <sortCondition descending="1" ref="B1:B280"/>
-    </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>